<commit_message>
add one new test case :"Set As Default Dashboard: Removing default dashboard"
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/Set_As_Default_Dashboard_NewUI_Content/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/Set_As_Default_Dashboard_NewUI_Content/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{CE39BE62-A321-48C6-9091-8EDA1278910B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{4088FE11-3579-4FB6-B272-E476EAFF8AEB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7125" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19185" windowHeight="3750" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>Variable</t>
   </si>
@@ -159,9 +159,6 @@
     <t>MicrosoftEdge</t>
   </si>
   <si>
-    <t>C82144 : Chrome: Set As Default Dashboard: Testing that the icon is displayed in the dashboard</t>
-  </si>
-  <si>
     <t>Automation_Analyzer</t>
   </si>
   <si>
@@ -181,6 +178,15 @@
   </si>
   <si>
     <t>Automation_Dashboard_Set_As_Default_Dashboard_Pin_work_check</t>
+  </si>
+  <si>
+    <t>C82179 Chrome: Testing that when hovering over "Set as default" tooltip says: 'Set as Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C82144 : Chrome: Set As Default Dashboard: Testing that the icon is displayed in the dashboard </t>
+  </si>
+  <si>
+    <t>Set_As_Default_Dashboard_Pin_tooltip</t>
   </si>
 </sst>
 </file>
@@ -646,7 +652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
@@ -1134,7 +1140,7 @@
         <v>33</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>34</v>
@@ -1168,7 +1174,7 @@
         <v>35</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>34</v>
@@ -1197,12 +1203,12 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
     </row>
-    <row r="17" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
@@ -1227,12 +1233,12 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
     </row>
-    <row r="18" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>48</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>49</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
@@ -1264,7 +1270,7 @@
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -1291,10 +1297,10 @@
     </row>
     <row r="20" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="6"/>
@@ -1385,9 +1391,44 @@
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
     </row>
-    <row r="23" spans="1:26" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="7"/>
+    <row r="23" spans="1:26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="3"/>
+    </row>
+    <row r="24" spans="1:26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="5"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
@@ -2738,7 +2779,7 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="A31:C31"/>
     <mergeCell ref="A2:C2"/>
@@ -2746,6 +2787,7 @@
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A23:C23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
add New Test cases for SetAsDefaultDashboard Section
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/Set_As_Default_Dashboard_NewUI_Content/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/Set_As_Default_Dashboard_NewUI_Content/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{4088FE11-3579-4FB6-B272-E476EAFF8AEB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0503BB63-BA01-4FDE-848A-5BE1D534819B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19185" windowHeight="3750" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20805" windowHeight="6195" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="66">
   <si>
     <t>Variable</t>
   </si>
@@ -187,6 +187,39 @@
   </si>
   <si>
     <t>Set_As_Default_Dashboard_Pin_tooltip</t>
+  </si>
+  <si>
+    <t>C82147 Chrome: Set As Default Dashboard : Setting two dashboards as default</t>
+  </si>
+  <si>
+    <t>Set_Default_Dashboard_1</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_SetDefault_Dashboard_One</t>
+  </si>
+  <si>
+    <t>Set_Default_Dashboard_2</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_SetDefault_Dashboard_Two</t>
+  </si>
+  <si>
+    <t>Automation_Analyzer2</t>
+  </si>
+  <si>
+    <t>automation_analyzer3</t>
+  </si>
+  <si>
+    <t>automation_analyzer4</t>
+  </si>
+  <si>
+    <t>automation_analyzer5</t>
+  </si>
+  <si>
+    <t>Set_Default_Dashboard_permission</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_Shared_View_Share_Edit</t>
   </si>
 </sst>
 </file>
@@ -650,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,10 +1144,18 @@
       <c r="C14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="D14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -1145,10 +1186,18 @@
       <c r="C15" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="D15" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -1179,10 +1228,18 @@
       <c r="C16" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
+      <c r="D16" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
@@ -1203,7 +1260,7 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
     </row>
-    <row r="17" spans="1:26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
@@ -1233,7 +1290,7 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
     </row>
-    <row r="18" spans="1:26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>47</v>
       </c>
@@ -1265,7 +1322,7 @@
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
     </row>
-    <row r="19" spans="1:26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -1391,7 +1448,7 @@
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
     </row>
-    <row r="23" spans="1:26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
@@ -1421,7 +1478,7 @@
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
     </row>
-    <row r="24" spans="1:26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>54</v>
       </c>
@@ -1453,20 +1510,24 @@
       <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
     </row>
-    <row r="25" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="5"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
+    <row r="25" spans="1:26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
       <c r="R25" s="3"/>
@@ -1479,22 +1540,26 @@
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
     </row>
-    <row r="26" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
+    <row r="26" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
       <c r="R26" s="3"/>
@@ -1507,9 +1572,13 @@
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
     </row>
-    <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
+    <row r="27" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="C27" s="5"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
@@ -1535,7 +1604,7 @@
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
     </row>
-    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
@@ -1563,9 +1632,13 @@
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
     </row>
-    <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="5"/>
-      <c r="B29" s="7"/>
+    <row r="29" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>65</v>
+      </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -1591,8 +1664,8 @@
       <c r="Y29" s="3"/>
       <c r="Z29" s="3"/>
     </row>
-    <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="7"/>
+    <row r="30" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="5"/>
       <c r="B30" s="7"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -1619,7 +1692,7 @@
       <c r="Y30" s="3"/>
       <c r="Z30" s="3"/>
     </row>
-    <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
@@ -1647,7 +1720,7 @@
       <c r="Y31" s="3"/>
       <c r="Z31" s="3"/>
     </row>
-    <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1675,7 +1748,7 @@
       <c r="Y32" s="3"/>
       <c r="Z32" s="3"/>
     </row>
-    <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="6"/>
@@ -1703,7 +1776,7 @@
       <c r="Y33" s="3"/>
       <c r="Z33" s="3"/>
     </row>
-    <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="6"/>
@@ -1731,7 +1804,7 @@
       <c r="Y34" s="3"/>
       <c r="Z34" s="3"/>
     </row>
-    <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="6"/>
@@ -1759,7 +1832,7 @@
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
     </row>
-    <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="3"/>
@@ -1787,7 +1860,7 @@
       <c r="Y36" s="3"/>
       <c r="Z36" s="3"/>
     </row>
-    <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="3"/>
@@ -1815,969 +1888,984 @@
       <c r="Y37" s="3"/>
       <c r="Z37" s="3"/>
     </row>
-    <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="974" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="975" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="976" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="977" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="978" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="979" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="980" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="981" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="982" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="983" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="984" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="985" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="986" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="987" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="988" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="989" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="990" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="991" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="994" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="995" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="996" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="997" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="998" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="999" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1000" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" spans="1:26" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A28:C28"/>
@@ -2786,7 +2874,7 @@
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A25:C25"/>
     <mergeCell ref="A23:C23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
SetAsDefaultDashboard Tenant test data
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/Set_As_Default_Dashboard_NewUI_Content/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/Set_As_Default_Dashboard_NewUI_Content/TestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0503BB63-BA01-4FDE-848A-5BE1D534819B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{8D98593D-EE71-4C37-9FF3-46C2470FD926}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20805" windowHeight="6195" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22155" windowHeight="5415" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="68">
   <si>
     <t>Variable</t>
   </si>
@@ -120,15 +120,9 @@
     <t>Tenant</t>
   </si>
   <si>
-    <t>demo</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
-    <t>admin</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
@@ -159,27 +153,15 @@
     <t>MicrosoftEdge</t>
   </si>
   <si>
-    <t>Automation_Analyzer</t>
-  </si>
-  <si>
-    <t>Automation_Analyzer1</t>
-  </si>
-  <si>
     <t>Set_As_Default_Dashboard_Pin_Displayed</t>
   </si>
   <si>
-    <t>Automation_Dashboard_Set_As_Default_Dashboard_Pin_Check</t>
-  </si>
-  <si>
     <t>C82145 - Chrome: Set As Default Dashboard: Testing that the icon is displayed in the dashboard and work correctly</t>
   </si>
   <si>
     <t>Set_As_Default_Dashboard_Pin_Work</t>
   </si>
   <si>
-    <t>Automation_Dashboard_Set_As_Default_Dashboard_Pin_work_check</t>
-  </si>
-  <si>
     <t>C82179 Chrome: Testing that when hovering over "Set as default" tooltip says: 'Set as Default</t>
   </si>
   <si>
@@ -204,22 +186,46 @@
     <t>Automation_Dashboard_SetDefault_Dashboard_Two</t>
   </si>
   <si>
-    <t>Automation_Analyzer2</t>
-  </si>
-  <si>
-    <t>automation_analyzer3</t>
-  </si>
-  <si>
-    <t>automation_analyzer4</t>
-  </si>
-  <si>
-    <t>automation_analyzer5</t>
-  </si>
-  <si>
     <t>Set_Default_Dashboard_permission</t>
   </si>
   <si>
     <t>Automation_Dashboard_Shared_View_Share_Edit</t>
+  </si>
+  <si>
+    <t>Automation_Analyzer_DefaultDB</t>
+  </si>
+  <si>
+    <t>Automation_analyzer_ShareDB</t>
+  </si>
+  <si>
+    <t>Automation_analyzer_EditDB</t>
+  </si>
+  <si>
+    <t>Automation_analyzer_ViewDB</t>
+  </si>
+  <si>
+    <t>Automation_analyzer_removeDefaultDB</t>
+  </si>
+  <si>
+    <t>Automation_Analyzer_checkDB</t>
+  </si>
+  <si>
+    <t>Automation_SetAsDefault_DashboardPin_Check</t>
+  </si>
+  <si>
+    <t>C82146 - Chrome:Set As Default Dashboard: Removing default dashboard</t>
+  </si>
+  <si>
+    <t>Set_As_Default_Dashboard_Pin_Remove</t>
+  </si>
+  <si>
+    <t>Automation_SetAsDefault_DashboardPin_Remove</t>
+  </si>
+  <si>
+    <t>Automation_analyzer_SetTwoDefaultDB</t>
+  </si>
+  <si>
+    <t>content_test</t>
   </si>
 </sst>
 </file>
@@ -683,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,8 +703,8 @@
     <col min="4" max="4" width="42.7109375" customWidth="1"/>
     <col min="5" max="5" width="28.28515625" customWidth="1"/>
     <col min="6" max="6" width="37.85546875" customWidth="1"/>
-    <col min="7" max="7" width="28.85546875" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="40.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
     <col min="9" max="9" width="27.5703125" customWidth="1"/>
     <col min="10" max="10" width="33.28515625" customWidth="1"/>
     <col min="11" max="15" width="8.5703125" customWidth="1"/>
@@ -1139,25 +1145,26 @@
         <v>31</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+        <v>67</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="J14" s="5"/>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
@@ -1178,28 +1185,29 @@
     </row>
     <row r="15" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+      <c r="H15" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="J15" s="5"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
@@ -1220,28 +1228,29 @@
     </row>
     <row r="16" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="D16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
+      <c r="H16" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="J16" s="5"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
@@ -1265,7 +1274,7 @@
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
@@ -1292,10 +1301,10 @@
     </row>
     <row r="18" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
@@ -1327,7 +1336,7 @@
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -1354,10 +1363,10 @@
     </row>
     <row r="20" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="6"/>
@@ -1386,10 +1395,10 @@
     </row>
     <row r="21" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
@@ -1416,12 +1425,12 @@
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
     </row>
-    <row r="22" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="6"/>
@@ -1448,12 +1457,12 @@
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
     </row>
-    <row r="23" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="4" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
@@ -1478,14 +1487,14 @@
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
     </row>
-    <row r="24" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="5"/>
+        <v>64</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="7"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
@@ -1515,7 +1524,7 @@
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="4" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
@@ -1540,12 +1549,12 @@
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
     </row>
-    <row r="26" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>57</v>
+        <v>48</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>62</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="6"/>
@@ -1572,26 +1581,24 @@
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
     </row>
-    <row r="27" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
+    <row r="27" spans="1:26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
@@ -1605,21 +1612,25 @@
       <c r="Z27" s="3"/>
     </row>
     <row r="28" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
+      <c r="A28" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
       <c r="P28" s="3"/>
       <c r="Q28" s="3"/>
       <c r="R28" s="3"/>
@@ -1634,24 +1645,24 @@
     </row>
     <row r="29" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
+        <v>52</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
       <c r="P29" s="3"/>
       <c r="Q29" s="3"/>
       <c r="R29" s="3"/>
@@ -1665,21 +1676,21 @@
       <c r="Z29" s="3"/>
     </row>
     <row r="30" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="5"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
       <c r="P30" s="3"/>
       <c r="Q30" s="3"/>
       <c r="R30" s="3"/>
@@ -1693,21 +1704,25 @@
       <c r="Z30" s="3"/>
     </row>
     <row r="31" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
+      <c r="A31" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
       <c r="P31" s="3"/>
       <c r="Q31" s="3"/>
       <c r="R31" s="3"/>
@@ -1721,21 +1736,21 @@
       <c r="Z31" s="3"/>
     </row>
     <row r="32" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="7"/>
-      <c r="B32" s="3"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="7"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
       <c r="P32" s="3"/>
       <c r="Q32" s="3"/>
       <c r="R32" s="3"/>
@@ -1749,21 +1764,21 @@
       <c r="Z32" s="3"/>
     </row>
     <row r="33" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
       <c r="P33" s="3"/>
       <c r="Q33" s="3"/>
       <c r="R33" s="3"/>
@@ -1777,9 +1792,9 @@
       <c r="Z33" s="3"/>
     </row>
     <row r="34" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="6"/>
+      <c r="A34" s="7"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
@@ -1833,21 +1848,21 @@
       <c r="Z35" s="3"/>
     </row>
     <row r="36" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="3"/>
-      <c r="O36" s="3"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
       <c r="P36" s="3"/>
       <c r="Q36" s="3"/>
       <c r="R36" s="3"/>
@@ -1861,21 +1876,21 @@
       <c r="Z36" s="3"/>
     </row>
     <row r="37" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="3"/>
-      <c r="O37" s="3"/>
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
       <c r="P37" s="3"/>
       <c r="Q37" s="3"/>
       <c r="R37" s="3"/>
@@ -1889,23 +1904,77 @@
       <c r="Z37" s="3"/>
     </row>
     <row r="38" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="3"/>
+      <c r="R38" s="3"/>
+      <c r="S38" s="3"/>
+      <c r="T38" s="3"/>
+      <c r="U38" s="3"/>
+      <c r="V38" s="3"/>
+      <c r="W38" s="3"/>
+      <c r="X38" s="3"/>
+      <c r="Y38" s="3"/>
+      <c r="Z38" s="3"/>
+    </row>
+    <row r="39" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="3"/>
+      <c r="T39" s="3"/>
+      <c r="U39" s="3"/>
+      <c r="V39" s="3"/>
+      <c r="W39" s="3"/>
+      <c r="X39" s="3"/>
+      <c r="Y39" s="3"/>
+      <c r="Z39" s="3"/>
+    </row>
+    <row r="40" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B41" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2865,15 +2934,19 @@
     <row r="998" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1001" spans="1:26" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1002" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1003" spans="1:26" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1004" spans="1:26" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A31:C31"/>
+  <mergeCells count="9">
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A33:C33"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A27:C27"/>
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="A23:C23"/>
   </mergeCells>
@@ -2897,7 +2970,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -2912,7 +2985,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -2927,7 +3000,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -2942,7 +3015,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -2957,7 +3030,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>

</xml_diff>

<commit_message>
SetAsDefault Dashboard latest updates to some functions in POM file
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/Set_As_Default_Dashboard_NewUI_Content/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/Set_As_Default_Dashboard_NewUI_Content/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{8D98593D-EE71-4C37-9FF3-46C2470FD926}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{5C6A5F06-2B19-4BBC-A095-04BF5DACC967}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22155" windowHeight="5415" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14595" windowHeight="4635" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -691,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
remove duplicate testcases and there testclass
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/Set_As_Default_Dashboard_NewUI_Content/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/Set_As_Default_Dashboard_NewUI_Content/TestData.xlsx
@@ -1,9 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{5C6A5F06-2B19-4BBC-A095-04BF5DACC967}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AFarid\git\qa\src\test\resources\TestDataFiles\Set_As_Default_Dashboard_NewUI_Content\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F14900C-44D9-448A-B393-7958682A4889}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14595" windowHeight="4635" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +17,6 @@
     <sheet name="Lists" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -22,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="69">
   <si>
     <t>Variable</t>
   </si>
@@ -226,6 +230,9 @@
   </si>
   <si>
     <t>content_test</t>
+  </si>
+  <si>
+    <t>admin</t>
   </si>
 </sst>
 </file>
@@ -689,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1004"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,6 +1172,9 @@
       <c r="H14" s="5" t="s">
         <v>67</v>
       </c>
+      <c r="I14" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="J14" s="5"/>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
@@ -1208,6 +1218,9 @@
       <c r="H15" s="5" t="s">
         <v>66</v>
       </c>
+      <c r="I15" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="J15" s="5"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
@@ -1250,6 +1263,9 @@
       </c>
       <c r="H16" s="5" t="s">
         <v>66</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>68</v>
       </c>
       <c r="J16" s="5"/>
       <c r="K16" s="6"/>
@@ -1425,7 +1441,7 @@
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
     </row>
-    <row r="22" spans="1:26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>36</v>
       </c>
@@ -1457,7 +1473,7 @@
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
     </row>
-    <row r="23" spans="1:26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
@@ -1487,7 +1503,7 @@
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
     </row>
-    <row r="24" spans="1:26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>64</v>
       </c>
@@ -1519,7 +1535,7 @@
       <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
     </row>
-    <row r="25" spans="1:26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
@@ -1549,7 +1565,7 @@
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
     </row>
-    <row r="26" spans="1:26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>48</v>
       </c>
@@ -1581,7 +1597,7 @@
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
     </row>
-    <row r="27" spans="1:26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -1611,7 +1627,7 @@
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
     </row>
-    <row r="28" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>50</v>
       </c>
@@ -1643,7 +1659,7 @@
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
     </row>
-    <row r="29" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>52</v>
       </c>
@@ -1675,7 +1691,7 @@
       <c r="Y29" s="3"/>
       <c r="Z29" s="3"/>
     </row>
-    <row r="30" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
@@ -1703,7 +1719,7 @@
       <c r="Y30" s="3"/>
       <c r="Z30" s="3"/>
     </row>
-    <row r="31" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>54</v>
       </c>
@@ -1735,7 +1751,7 @@
       <c r="Y31" s="3"/>
       <c r="Z31" s="3"/>
     </row>
-    <row r="32" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="7"/>
       <c r="C32" s="3"/>
@@ -1763,7 +1779,7 @@
       <c r="Y32" s="3"/>
       <c r="Z32" s="3"/>
     </row>
-    <row r="33" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
@@ -1791,7 +1807,7 @@
       <c r="Y33" s="3"/>
       <c r="Z33" s="3"/>
     </row>
-    <row r="34" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1819,7 +1835,7 @@
       <c r="Y34" s="3"/>
       <c r="Z34" s="3"/>
     </row>
-    <row r="35" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="6"/>
@@ -1847,7 +1863,7 @@
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
     </row>
-    <row r="36" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="6"/>
@@ -1875,7 +1891,7 @@
       <c r="Y36" s="3"/>
       <c r="Z36" s="3"/>
     </row>
-    <row r="37" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="6"/>
@@ -1903,7 +1919,7 @@
       <c r="Y37" s="3"/>
       <c r="Z37" s="3"/>
     </row>
-    <row r="38" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="3"/>
@@ -1931,7 +1947,7 @@
       <c r="Y38" s="3"/>
       <c r="Z38" s="3"/>
     </row>
-    <row r="39" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="3"/>
@@ -1959,7 +1975,7 @@
       <c r="Y39" s="3"/>
       <c r="Z39" s="3"/>
     </row>
-    <row r="40" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>34</v>
       </c>
@@ -1967,7 +1983,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>36</v>
       </c>
@@ -1975,969 +1991,967 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="137" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="138" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="139" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="140" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="141" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="142" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="143" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="144" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="146" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="147" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="162" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="164" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="165" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="167" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="168" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="169" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="170" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="171" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="172" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="173" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="174" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="175" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="177" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="178" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="179" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="180" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="181" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="182" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="183" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="184" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="185" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="186" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="187" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="188" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="189" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="190" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="191" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="192" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="193" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="194" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="195" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="196" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="197" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="198" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="199" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="200" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="201" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="202" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="203" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="204" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="205" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="206" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="207" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="208" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="209" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="210" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="211" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="212" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="213" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="214" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="215" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="216" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="217" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="218" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="219" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="220" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="221" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="222" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="223" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="224" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="225" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="226" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="227" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="228" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="229" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="230" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="231" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="232" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="233" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="234" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="235" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="236" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="237" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="238" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="239" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="240" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="241" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="242" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="243" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="244" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="245" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="246" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="247" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="248" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="249" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="250" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="251" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="252" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="253" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="254" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="255" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="256" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="257" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="258" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="259" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="260" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="261" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="262" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="263" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="264" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="265" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="266" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="267" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="268" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="269" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="270" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="271" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="272" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="273" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="274" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="275" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="276" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="277" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="278" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="279" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="280" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="281" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="282" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="283" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="284" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="285" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="286" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="287" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="288" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="289" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="290" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="291" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="292" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="293" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="294" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="295" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="296" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="297" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="298" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="299" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="300" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="301" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="302" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="303" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="304" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="305" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="306" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="307" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="308" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="309" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="310" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="311" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="312" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="313" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="314" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="315" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="316" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="317" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="318" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="319" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="320" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="321" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="322" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="323" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="324" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="325" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="326" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="327" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="328" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="329" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="330" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="331" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="332" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="333" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="334" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="335" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="336" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="337" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="338" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="339" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="340" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="341" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="342" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="343" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="344" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="345" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="346" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="347" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="348" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="349" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="350" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="351" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="352" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="353" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="354" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="355" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="356" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="357" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="358" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="359" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="360" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="361" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="362" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="363" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="364" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="365" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="366" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="367" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="368" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="369" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="370" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="371" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="372" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="373" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="374" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="375" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="376" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="377" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="378" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="379" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="380" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="381" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="382" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="383" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="384" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="385" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="386" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="387" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="388" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="389" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="390" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="391" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="392" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="393" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="394" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="395" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="396" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="397" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="398" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="399" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="400" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="401" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="402" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="403" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="404" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="405" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="406" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="407" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="408" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="409" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="410" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="411" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="412" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="413" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="414" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="415" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="416" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="417" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="418" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="419" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="420" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="421" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="422" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="423" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="424" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="425" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="426" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="427" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="428" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="429" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="430" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="431" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="432" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="433" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="434" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="435" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="436" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="437" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="438" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="439" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="440" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="441" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="442" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="443" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="444" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="445" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="446" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="447" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="448" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="449" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="450" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="451" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="452" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="453" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="454" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="455" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="456" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="457" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="458" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="459" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="460" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="461" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="462" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="463" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="464" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="465" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="466" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="467" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="468" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="469" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="470" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="471" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="472" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="473" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="474" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="475" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="476" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="477" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="478" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="480" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="481" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="482" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="483" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="484" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="485" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="486" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="487" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="488" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="489" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="490" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="491" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="492" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="493" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="494" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="495" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="496" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="497" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="498" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="499" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="500" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="501" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="502" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="503" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="504" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="505" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="506" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="507" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="508" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="509" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="510" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="511" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="512" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="513" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="514" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="515" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="516" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="517" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="518" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="519" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="520" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="521" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="522" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="523" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="524" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="525" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="526" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="527" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="528" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="529" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="530" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="531" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="532" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="533" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="534" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="535" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="536" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="537" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="538" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="539" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="540" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="541" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="542" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="543" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="544" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="545" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="546" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="547" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="548" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="549" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="550" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="551" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="552" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="553" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="554" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="555" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="556" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="557" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="558" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="559" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="560" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="561" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="562" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="563" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="564" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="565" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="566" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="567" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="568" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="569" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="570" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="571" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="572" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="573" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="574" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="575" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="576" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="577" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="578" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="579" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="580" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="581" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="582" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="583" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="584" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="585" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="586" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="587" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="588" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="589" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="590" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="591" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="592" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="593" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="594" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="595" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="596" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="597" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="598" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="599" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="600" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="601" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="602" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="603" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="604" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="605" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="606" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="607" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="608" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="609" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="610" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="611" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="612" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="613" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="614" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="615" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="616" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="617" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="618" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="619" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="620" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="621" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="622" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="623" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="624" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="625" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="626" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="627" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="628" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="629" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="630" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="631" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="632" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="633" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="634" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="635" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="636" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="637" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="638" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="639" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="640" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="641" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="642" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="643" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="644" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="645" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="646" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="647" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="648" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="649" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="650" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="651" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="652" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="653" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="654" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="655" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="656" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="657" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="658" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="659" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="660" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="661" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="662" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="663" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="664" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="665" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="666" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="667" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="668" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="669" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="670" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="671" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="672" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="673" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="674" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="675" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="676" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="677" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="678" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="679" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="680" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="681" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="682" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="683" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="684" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="685" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="686" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="687" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="688" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="689" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="690" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="691" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="692" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="693" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="694" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="695" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="696" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="697" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="698" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="699" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="700" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="701" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="702" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="703" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="704" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="705" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="706" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="707" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="708" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="709" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="710" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="711" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="712" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="713" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="714" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="715" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="716" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="717" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="718" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="719" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="720" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="721" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="722" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="723" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="724" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="725" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="726" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="727" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="728" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="729" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="730" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="731" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="732" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="733" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="734" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="735" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="736" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="737" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="738" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="739" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="740" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="741" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="742" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="743" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="744" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="745" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="746" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="747" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="748" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="749" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="750" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="751" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="752" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="753" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="754" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="755" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="756" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="757" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="758" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="759" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="760" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="761" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="762" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="763" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="764" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="765" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="766" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="767" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="768" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="769" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="770" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="771" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="772" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="773" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="774" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="775" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="776" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="777" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="778" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="779" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="780" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="781" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="782" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="783" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="784" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="785" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="786" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="787" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="788" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="789" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="790" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="791" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="792" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="793" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="794" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="795" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="796" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="797" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="798" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="799" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="800" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="801" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="802" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="803" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="804" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="805" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="806" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="807" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="808" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="809" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="810" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="811" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="812" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="813" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="814" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="815" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="816" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="817" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="818" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="819" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="820" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="821" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="822" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="823" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="824" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="825" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="826" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="827" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="828" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="829" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="830" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="831" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="832" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="833" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="834" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="835" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="836" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="837" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="838" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="839" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="840" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="841" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="842" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="843" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="844" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="845" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="846" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="847" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="848" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="849" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="850" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="851" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="852" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="853" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="854" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="855" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="856" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="857" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="858" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="859" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="860" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="861" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="862" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="863" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="864" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="865" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="866" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="867" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="868" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="869" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="870" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="871" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="872" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="873" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="874" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="875" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="876" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="877" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="878" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="879" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="880" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="881" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="882" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="883" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="884" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="885" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="886" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="887" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="888" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="889" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="890" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="891" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="892" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="893" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="894" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="895" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="896" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="897" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="898" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="899" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="900" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="901" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="902" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="903" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="904" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="905" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="906" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="907" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="908" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="909" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="910" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="911" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="912" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="913" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="914" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="915" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="916" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="917" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="918" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="919" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="920" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="921" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="922" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="923" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="924" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="925" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="926" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="927" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="928" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="929" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="930" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="931" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="932" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="933" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="934" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="935" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="936" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="937" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="938" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="939" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="940" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="941" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="942" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="943" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="944" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="945" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="946" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="947" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="948" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="949" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="950" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="951" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="952" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="953" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="954" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="955" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="956" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="957" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="958" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="959" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="960" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="961" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="962" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="963" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="964" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="965" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="966" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="967" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="968" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="969" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="970" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="971" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="972" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="973" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="974" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="975" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="976" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="977" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="978" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="979" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="980" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="981" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="982" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="983" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="984" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="985" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="986" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="987" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="988" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="989" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="990" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="991" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="992" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="993" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="994" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="995" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="996" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="997" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="998" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1001" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1002" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1003" spans="1:26" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1004" spans="1:26" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="A30:C30"/>

</xml_diff>

<commit_message>
update tenant name in TestData File from Content test to content
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/Set_As_Default_Dashboard_NewUI_Content/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/Set_As_Default_Dashboard_NewUI_Content/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AFarid\git\qa\src\test\resources\TestDataFiles\Set_As_Default_Dashboard_NewUI_Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F14900C-44D9-448A-B393-7958682A4889}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E7E751-762D-4BF5-A91A-0ABCF354D48C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14595" windowHeight="4635" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -229,10 +229,10 @@
     <t>Automation_analyzer_SetTwoDefaultDB</t>
   </si>
   <si>
-    <t>content_test</t>
-  </si>
-  <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t>content</t>
   </si>
 </sst>
 </file>
@@ -698,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1152,28 +1152,28 @@
         <v>31</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J14" s="5"/>
       <c r="K14" s="6"/>
@@ -1219,7 +1219,7 @@
         <v>66</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J15" s="5"/>
       <c r="K15" s="6"/>
@@ -1265,7 +1265,7 @@
         <v>66</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J16" s="5"/>
       <c r="K16" s="6"/>

</xml_diff>